<commit_message>
Updated docs with reduced pipeline complexity
</commit_message>
<xml_diff>
--- a/conversation/conversation.xlsx
+++ b/conversation/conversation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Downloads/conversation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Projects/aws/planet-money-generator/conversation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EF460E-E570-514C-8889-FC899F0CBB24}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145A6D02-F890-6B4E-9871-75025B3927C6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="1180" windowWidth="38400" windowHeight="21140" xr2:uid="{CEC2C03D-29C6-4143-8FDA-B0EFDCEE1138}"/>
   </bookViews>
@@ -87,58 +87,58 @@
     <t xml:space="preserve">Yeah. And it's not true. And they don't create a lot of the political as what I haven to the Norwegian Geological results from the oil companies exploring to Martin Sandbu wrote. Martin Sandbu wrote. Martin Sandbu wrote. Martin Sandbu - we're only going to be very, very, very powerful with </t>
   </si>
   <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/pollyc203fe83-ab46-c547-d1d4-78590bb7a9e3.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly0b17984f-1ce7-dcbb-fe1a-b053890b0adc.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly6a2c8e95-5ce8-aa8a-a79d-230636ec7ee2.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly0007f4e2-25fb-a836-67a8-4eacd4eaaf5b.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly4fb20910-11c6-4021-0f67-1fa197fbb45c.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/pollye8366795-e413-2b1d-adbc-61e4bc099055.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly6f1246d7-123f-7368-c815-83c65ce8664a.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly7c1545c8-381d-9bee-a6b7-7535b70fc1f7.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/pollyf00a797d-fcce-3afd-36ad-4e60325f50cf.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly8eb39730-e2ad-c9e7-b16d-7b57d5c6a040.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/pollyf116fcb8-3cb5-9e7d-1f2f-7b41a73cac19.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly67507cd2-7339-5782-5f56-976b7121ab52.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/pollybe496aab-21d3-d6e1-4301-4d57307c6be8.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly797a107a-b8c4-eb2c-8a39-1ae27351878e.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/pollydf8470b8-4638-8d8b-e4eb-7281a90512d1.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/pollyfbbb2c05-587e-2eeb-1526-00ed119f1ec3.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/polly5e451b99-61ed-24f5-e92c-feddae992629.mp3</t>
-  </si>
-  <si>
-    <t>https://planey-money-generator.s3.amazonaws.com/pollyf9d350be-fd35-ec6d-ee5e-887749082bd7.mp3</t>
+    <t>pollyc203fe83-ab46-c547-d1d4-78590bb7a9e3.mp3</t>
+  </si>
+  <si>
+    <t>pollyf116fcb8-3cb5-9e7d-1f2f-7b41a73cac19.mp3</t>
+  </si>
+  <si>
+    <t>polly0b17984f-1ce7-dcbb-fe1a-b053890b0adc.mp3</t>
+  </si>
+  <si>
+    <t>polly67507cd2-7339-5782-5f56-976b7121ab52.mp3</t>
+  </si>
+  <si>
+    <t>polly6a2c8e95-5ce8-aa8a-a79d-230636ec7ee2.mp3</t>
+  </si>
+  <si>
+    <t>pollybe496aab-21d3-d6e1-4301-4d57307c6be8.mp3</t>
+  </si>
+  <si>
+    <t>polly0007f4e2-25fb-a836-67a8-4eacd4eaaf5b.mp3</t>
+  </si>
+  <si>
+    <t>polly797a107a-b8c4-eb2c-8a39-1ae27351878e.mp3</t>
+  </si>
+  <si>
+    <t>polly4fb20910-11c6-4021-0f67-1fa197fbb45c.mp3</t>
+  </si>
+  <si>
+    <t>pollydf8470b8-4638-8d8b-e4eb-7281a90512d1.mp3</t>
+  </si>
+  <si>
+    <t>pollye8366795-e413-2b1d-adbc-61e4bc099055.mp3</t>
+  </si>
+  <si>
+    <t>pollyfbbb2c05-587e-2eeb-1526-00ed119f1ec3.mp3</t>
+  </si>
+  <si>
+    <t>polly6f1246d7-123f-7368-c815-83c65ce8664a.mp3</t>
+  </si>
+  <si>
+    <t>polly5e451b99-61ed-24f5-e92c-feddae992629.mp3</t>
+  </si>
+  <si>
+    <t>polly7c1545c8-381d-9bee-a6b7-7535b70fc1f7.mp3</t>
+  </si>
+  <si>
+    <t>pollyf9d350be-fd35-ec6d-ee5e-887749082bd7.mp3</t>
+  </si>
+  <si>
+    <t>polly8eb39730-e2ad-c9e7-b16d-7b57d5c6a040.mp3</t>
+  </si>
+  <si>
+    <t>pollyf00a797d-fcce-3afd-36ad-4e60325f50cf.mp3</t>
   </si>
 </sst>
 </file>
@@ -512,14 +512,14 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.5" customWidth="1"/>
+    <col min="3" max="3" width="94.1640625" customWidth="1"/>
     <col min="4" max="4" width="58.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -534,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -562,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -576,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -590,7 +590,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -604,7 +604,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -618,7 +618,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -632,7 +632,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -646,7 +646,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -674,7 +674,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -702,7 +702,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -716,7 +716,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -730,7 +730,7 @@
         <v>16</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -744,7 +744,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -758,7 +758,7 @@
         <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -772,27 +772,27 @@
         <v>19</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{E3C8594E-0E2A-F64F-82A4-DF0AD012B121}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{A2588531-F121-FB49-AE79-27AD197B43D6}"/>
-    <hyperlink ref="D10" r:id="rId3" xr:uid="{47E8303D-6EEB-D548-88EB-028E2C808823}"/>
-    <hyperlink ref="D12" r:id="rId4" xr:uid="{926A7AFE-58D7-5149-B3A8-23115A591F94}"/>
-    <hyperlink ref="D14" r:id="rId5" xr:uid="{27394DDA-3C27-334A-A53B-4174AF8C0D4F}"/>
-    <hyperlink ref="D16" r:id="rId6" xr:uid="{0FCAF2AB-A9D0-5D4A-B2A8-1BEF732012CC}"/>
-    <hyperlink ref="D1" r:id="rId7" xr:uid="{741C8258-01B5-8641-BF33-4B04B3F1930C}"/>
-    <hyperlink ref="D18" r:id="rId8" xr:uid="{44B3EF18-CA68-6942-AE8C-5DC2DB904405}"/>
-    <hyperlink ref="D3" r:id="rId9" xr:uid="{91993D89-1A8B-CE48-B987-D39C91D14BE5}"/>
-    <hyperlink ref="D5" r:id="rId10" xr:uid="{F5C4536C-E86E-194B-915A-FE7739B12CC0}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{818ED3B6-AC01-3D4D-89F7-C97BC7FDFEC6}"/>
-    <hyperlink ref="D9" r:id="rId12" xr:uid="{23414580-BFF1-074E-A033-6ED3FB1D8636}"/>
-    <hyperlink ref="D11" r:id="rId13" xr:uid="{CEED1A66-C157-254C-926A-7FF0BB4715AA}"/>
-    <hyperlink ref="D13" r:id="rId14" xr:uid="{8B1F83C9-644A-5747-A157-09E6BA7D4B08}"/>
-    <hyperlink ref="D15" r:id="rId15" xr:uid="{76640861-0BC3-DD4D-9166-3C8DDEECF6BB}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{F6DCBF0D-B7B7-714C-99E4-3ED7B5BE86B4}"/>
+    <hyperlink ref="D2" r:id="rId1" display="https://planey-money-generator.s3.amazonaws.com/pollyc203fe83-ab46-c547-d1d4-78590bb7a9e3.mp3" xr:uid="{E3C8594E-0E2A-F64F-82A4-DF0AD012B121}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://planey-money-generator.s3.amazonaws.com/polly0007f4e2-25fb-a836-67a8-4eacd4eaaf5b.mp3" xr:uid="{A2588531-F121-FB49-AE79-27AD197B43D6}"/>
+    <hyperlink ref="D10" r:id="rId3" display="https://planey-money-generator.s3.amazonaws.com/polly4fb20910-11c6-4021-0f67-1fa197fbb45c.mp3" xr:uid="{47E8303D-6EEB-D548-88EB-028E2C808823}"/>
+    <hyperlink ref="D12" r:id="rId4" display="https://planey-money-generator.s3.amazonaws.com/pollye8366795-e413-2b1d-adbc-61e4bc099055.mp3" xr:uid="{926A7AFE-58D7-5149-B3A8-23115A591F94}"/>
+    <hyperlink ref="D14" r:id="rId5" display="https://planey-money-generator.s3.amazonaws.com/polly6f1246d7-123f-7368-c815-83c65ce8664a.mp3" xr:uid="{27394DDA-3C27-334A-A53B-4174AF8C0D4F}"/>
+    <hyperlink ref="D16" r:id="rId6" display="https://planey-money-generator.s3.amazonaws.com/polly7c1545c8-381d-9bee-a6b7-7535b70fc1f7.mp3" xr:uid="{0FCAF2AB-A9D0-5D4A-B2A8-1BEF732012CC}"/>
+    <hyperlink ref="D1" r:id="rId7" display="https://planey-money-generator.s3.amazonaws.com/pollyf00a797d-fcce-3afd-36ad-4e60325f50cf.mp3" xr:uid="{741C8258-01B5-8641-BF33-4B04B3F1930C}"/>
+    <hyperlink ref="D18" r:id="rId8" display="https://planey-money-generator.s3.amazonaws.com/polly8eb39730-e2ad-c9e7-b16d-7b57d5c6a040.mp3" xr:uid="{44B3EF18-CA68-6942-AE8C-5DC2DB904405}"/>
+    <hyperlink ref="D3" r:id="rId9" display="https://planey-money-generator.s3.amazonaws.com/pollyf116fcb8-3cb5-9e7d-1f2f-7b41a73cac19.mp3" xr:uid="{91993D89-1A8B-CE48-B987-D39C91D14BE5}"/>
+    <hyperlink ref="D5" r:id="rId10" display="https://planey-money-generator.s3.amazonaws.com/polly67507cd2-7339-5782-5f56-976b7121ab52.mp3" xr:uid="{F5C4536C-E86E-194B-915A-FE7739B12CC0}"/>
+    <hyperlink ref="D7" r:id="rId11" display="https://planey-money-generator.s3.amazonaws.com/pollybe496aab-21d3-d6e1-4301-4d57307c6be8.mp3" xr:uid="{818ED3B6-AC01-3D4D-89F7-C97BC7FDFEC6}"/>
+    <hyperlink ref="D9" r:id="rId12" display="https://planey-money-generator.s3.amazonaws.com/polly797a107a-b8c4-eb2c-8a39-1ae27351878e.mp3" xr:uid="{23414580-BFF1-074E-A033-6ED3FB1D8636}"/>
+    <hyperlink ref="D11" r:id="rId13" display="https://planey-money-generator.s3.amazonaws.com/pollydf8470b8-4638-8d8b-e4eb-7281a90512d1.mp3" xr:uid="{CEED1A66-C157-254C-926A-7FF0BB4715AA}"/>
+    <hyperlink ref="D13" r:id="rId14" display="https://planey-money-generator.s3.amazonaws.com/pollyfbbb2c05-587e-2eeb-1526-00ed119f1ec3.mp3" xr:uid="{8B1F83C9-644A-5747-A157-09E6BA7D4B08}"/>
+    <hyperlink ref="D15" r:id="rId15" display="https://planey-money-generator.s3.amazonaws.com/polly5e451b99-61ed-24f5-e92c-feddae992629.mp3" xr:uid="{76640861-0BC3-DD4D-9166-3C8DDEECF6BB}"/>
+    <hyperlink ref="D17" r:id="rId16" display="https://planey-money-generator.s3.amazonaws.com/pollyf9d350be-fd35-ec6d-ee5e-887749082bd7.mp3" xr:uid="{F6DCBF0D-B7B7-714C-99E4-3ED7B5BE86B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>